<commit_message>
BUGS CAUGHT: user friendly excel sheet formatting allowed
</commit_message>
<xml_diff>
--- a/Book4.xlsx
+++ b/Book4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianmatzelle/Projects/string_sorting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5846DE8D-5CB7-BF49-A60B-E43B1A9F27B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA89B4D2-6F61-CE49-8370-CC997C2DC957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10840" yWindow="8620" windowWidth="34200" windowHeight="15220" xr2:uid="{A022BD7E-85EA-4F58-87F7-FDE614A74DC4}"/>
+    <workbookView xWindow="0" yWindow="7020" windowWidth="34200" windowHeight="15220" xr2:uid="{A022BD7E-85EA-4F58-87F7-FDE614A74DC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1023,909 +1023,909 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DACF668-4EB7-4B9F-8451-C18D166C7755}">
-  <dimension ref="A2:B157"/>
+  <dimension ref="A2:D157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
+      <c r="D21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
+      <c r="D37" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
+      <c r="D39" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" t="s">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B69" t="s">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B72" t="s">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B73" t="s">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D73" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B75" t="s">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B76" t="s">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B77" t="s">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B78" t="s">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B79" t="s">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D79" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B80" t="s">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D80" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B81" t="s">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D81" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" t="s">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D82" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B83" t="s">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D83" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B84" t="s">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B85" t="s">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B86" t="s">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D86" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B87" t="s">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D87" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D88" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D89" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B90" t="s">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D90" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B91" t="s">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D91" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B92" t="s">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B94" t="s">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B95" t="s">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D95" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B96" t="s">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D96" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B97" t="s">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B98" t="s">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B99" t="s">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B100" t="s">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B101" t="s">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B102" t="s">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D102" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B103" t="s">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D103" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B104" t="s">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D104" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B105" t="s">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D105" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B106" t="s">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D106" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B107" t="s">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D107" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B108" t="s">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D108" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B109" t="s">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D109" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B110" t="s">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D110" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B111" t="s">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D111" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B112" t="s">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D112" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B113" t="s">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D113" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B114" t="s">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D114" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B115" t="s">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D115" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B116" t="s">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D116" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B117" t="s">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D117" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B118" t="s">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D118" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B119" t="s">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D119" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B120" t="s">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D120" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B121" t="s">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D121" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B122" t="s">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D122" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B123" t="s">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D123" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B124" t="s">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D124" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B125" t="s">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D125" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B126" t="s">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D126" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B127" t="s">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D127" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B128" t="s">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D128" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B129" t="s">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D129" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B130" t="s">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D130" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B131" t="s">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D131" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B132" t="s">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D132" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B133" t="s">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D133" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B134" t="s">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D134" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B135" t="s">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D135" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B136" t="s">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D136" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B137" t="s">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D137" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B138" t="s">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D138" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B139" t="s">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D139" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B140" t="s">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B141" t="s">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D141" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B142" t="s">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D142" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B143" t="s">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D143" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B144" t="s">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D144" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B145" t="s">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D145" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B146" t="s">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D146" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B147" t="s">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D147" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B148" t="s">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D148" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B149" t="s">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D149" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B150" t="s">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D150" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B151" t="s">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D151" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B152" t="s">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D152" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B153" t="s">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D153" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B154" t="s">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D154" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B155" t="s">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D155" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B156" t="s">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D156" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B157" t="s">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D157" t="s">
         <v>191</v>
       </c>
     </row>

</xml_diff>